<commit_message>
snowdepth for all measurements and improved density visualization
</commit_message>
<xml_diff>
--- a/data/01-31-densitySLF.xlsx
+++ b/data/01-31-densitySLF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jille\Documents\Uni\Master-Mechatronik\Masterarbeit\Messung1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jille\Documents\Uni\Master-Mechatronik\Masterarbeit\SMP-SignalProcessing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C4FAE-E8B7-46FE-9E70-7035B8CD890E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4524DA1F-4FF9-4713-87D1-9C0D7D661543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{F87BFA84-DB09-4A4E-8E0E-1B2FD7CE4138}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F87BFA84-DB09-4A4E-8E0E-1B2FD7CE4138}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>snowdepth</t>
   </si>
@@ -44,10 +44,13 @@
     <t>density SLF in kg/m^3</t>
   </si>
   <si>
-    <t xml:space="preserve">density mean </t>
+    <t xml:space="preserve">density1 </t>
   </si>
   <si>
-    <t xml:space="preserve">density1 </t>
+    <t>snowheight</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -419,150 +422,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F56E685-F6ED-4C83-A160-21E3B800886C}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>28</v>
+      </c>
+      <c r="B5">
         <v>90</v>
       </c>
-      <c r="B4">
+      <c r="C5">
         <v>133</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>38</v>
+      </c>
+      <c r="B6">
         <v>80</v>
       </c>
-      <c r="B5">
+      <c r="C6">
         <v>138</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <v>554</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>48</v>
+      </c>
+      <c r="B7">
         <v>70</v>
       </c>
-      <c r="B6">
+      <c r="C7">
         <v>244</v>
       </c>
-      <c r="C6">
+      <c r="D7">
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>58</v>
+      </c>
+      <c r="B8">
         <v>60</v>
       </c>
-      <c r="B7">
+      <c r="C8">
         <v>279</v>
       </c>
-      <c r="C7">
+      <c r="D8">
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>68</v>
+      </c>
+      <c r="B9">
         <v>50</v>
       </c>
-      <c r="B8">
+      <c r="C9">
         <v>256</v>
       </c>
-      <c r="C8">
+      <c r="D9">
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>78</v>
+      </c>
+      <c r="B10">
         <v>40</v>
       </c>
-      <c r="B9">
+      <c r="C10">
         <v>296</v>
       </c>
-      <c r="C9">
+      <c r="D10">
         <v>296</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>88</v>
+      </c>
+      <c r="B11">
         <v>30</v>
       </c>
-      <c r="B10">
+      <c r="C11">
         <v>250</v>
       </c>
-      <c r="C10">
+      <c r="D11">
         <v>259</v>
       </c>
-      <c r="D10">
+      <c r="E11">
         <v>293</v>
       </c>
-      <c r="E10">
+      <c r="F11">
         <v>243</v>
       </c>
-      <c r="F10">
+      <c r="G11">
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>98</v>
+      </c>
+      <c r="B12">
         <v>20</v>
       </c>
-      <c r="B11">
+      <c r="C12">
         <v>246</v>
       </c>
-      <c r="C11">
+      <c r="D12">
         <v>239</v>
       </c>
-      <c r="D11">
+      <c r="E12">
         <v>253</v>
       </c>
     </row>

</xml_diff>